<commit_message>
added class to get information from a file, as well as made a folder to keep old version in
</commit_message>
<xml_diff>
--- a/testdoc.xlsx
+++ b/testdoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Normal-Ratio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBA80B5-2893-4941-A2FA-DBB8972A0FEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5669425C-034A-46EE-8990-A8F8E6881F4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D985AB9-BE62-4889-869A-26A05BB85C44}"/>
+    <workbookView xWindow="6195" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{6D985AB9-BE62-4889-869A-26A05BB85C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>N</t>
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -390,13 +402,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89348CE6-0474-4892-9DBC-DDDB46D9A76F}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -433,6 +448,74 @@
       </c>
       <c r="E2">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added FileInformation class and Estimate Class
</commit_message>
<xml_diff>
--- a/testdoc.xlsx
+++ b/testdoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Normal-Ratio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5669425C-034A-46EE-8990-A8F8E6881F4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA265E2D-41F8-49DC-8E60-D9A55012ED20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6195" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{6D985AB9-BE62-4889-869A-26A05BB85C44}"/>
   </bookViews>
@@ -405,12 +405,14 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -455,19 +457,19 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>-176.65</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>-149.8056</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>-148.9</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>149.11080000000001</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>150.00360000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -475,19 +477,19 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>51.883299999999998</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>61.188899999999997</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>61.716700000000003</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>60.958300000000001</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>61.216700000000003</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changed some data in the excel file
</commit_message>
<xml_diff>
--- a/testdoc.xlsx
+++ b/testdoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Normal-Ratio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\Profile\Downloads\estimates\Estimating-Missing-Climate-Values\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA265E2D-41F8-49DC-8E60-D9A55012ED20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEF47F2-E768-4645-A86A-7C72FA6E4F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="3150" windowWidth="21600" windowHeight="11385" xr2:uid="{6D985AB9-BE62-4889-869A-26A05BB85C44}"/>
+    <workbookView xWindow="20370" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{6D985AB9-BE62-4889-869A-26A05BB85C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,6 +451,9 @@
       <c r="E2">
         <v>4</v>
       </c>
+      <c r="F2">
+        <v>4.0999999999999996</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
added more methods as well as more variables
</commit_message>
<xml_diff>
--- a/testdoc.xlsx
+++ b/testdoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\Profile\Downloads\estimates\Estimating-Missing-Climate-Values\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Estimating-Missing-Climate-Values\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEF47F2-E768-4645-A86A-7C72FA6E4F8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F11BDD-3B9E-4B2C-B21C-04BF25C0101C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4680" windowWidth="29040" windowHeight="15840" xr2:uid="{6D985AB9-BE62-4889-869A-26A05BB85C44}"/>
+    <workbookView xWindow="2865" yWindow="2760" windowWidth="21600" windowHeight="11325" xr2:uid="{6D985AB9-BE62-4889-869A-26A05BB85C44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>N</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>ri</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89348CE6-0474-4892-9DBC-DDDB46D9A76F}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,19 +506,19 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>350</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>430</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>387</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -521,6 +527,46 @@
       </c>
       <c r="B6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>38</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>